<commit_message>
minor change for health index
</commit_message>
<xml_diff>
--- a/indice_sante_1/Explained_variance.xlsx
+++ b/indice_sante_1/Explained_variance.xlsx
@@ -384,13 +384,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4.36060453251903</v>
+        <v>4.612846683653662</v>
       </c>
       <c r="C2">
-        <v>9.277881984083059</v>
+        <v>9.413972823782968</v>
       </c>
       <c r="D2">
-        <v>9.277881984083059</v>
+        <v>9.413972823782968</v>
       </c>
     </row>
     <row r="3">
@@ -398,13 +398,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>11.40853372841415</v>
+        <v>9.981690992661678</v>
       </c>
       <c r="C3">
-        <v>13.2657368935048</v>
+        <v>18.48461294937369</v>
       </c>
       <c r="D3">
-        <v>13.2657368935048</v>
+        <v>18.48461294937369</v>
       </c>
     </row>
     <row r="4">
@@ -412,13 +412,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>11.75003878464795</v>
+        <v>10.21802379466729</v>
       </c>
       <c r="C4">
-        <v>14.50622072178759</v>
+        <v>16.48068353978608</v>
       </c>
       <c r="D4">
-        <v>14.50622072178759</v>
+        <v>16.48068353978608</v>
       </c>
     </row>
     <row r="5">
@@ -426,13 +426,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>11.40130998148398</v>
+        <v>10.18162570406218</v>
       </c>
       <c r="C5">
-        <v>12.52891206756482</v>
+        <v>16.16131064136858</v>
       </c>
       <c r="D5">
-        <v>12.52891206756482</v>
+        <v>16.16131064136858</v>
       </c>
     </row>
     <row r="6">
@@ -440,13 +440,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>11.45675287186818</v>
+        <v>10.29058658973594</v>
       </c>
       <c r="C6">
-        <v>15.91215676648368</v>
+        <v>14.70083798533697</v>
       </c>
       <c r="D6">
-        <v>15.91215676648368</v>
+        <v>14.70083798533697</v>
       </c>
     </row>
     <row r="7">
@@ -454,13 +454,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>14.49877030372815</v>
+        <v>10.09243780125401</v>
       </c>
       <c r="C7">
-        <v>16.2907531502563</v>
+        <v>14.41776828750572</v>
       </c>
       <c r="D7">
-        <v>16.2907531502563</v>
+        <v>14.41776828750572</v>
       </c>
     </row>
     <row r="8">
@@ -468,13 +468,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>13.42551026572693</v>
+        <v>10.0300599756187</v>
       </c>
       <c r="C8">
-        <v>14.91723362858546</v>
+        <v>13.73980818577903</v>
       </c>
       <c r="D8">
-        <v>14.91723362858546</v>
+        <v>13.73980818577903</v>
       </c>
     </row>
     <row r="9">
@@ -482,13 +482,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>13.6286065143117</v>
+        <v>10.10764763466389</v>
       </c>
       <c r="C9">
-        <v>15.48705285717237</v>
+        <v>13.84609265022454</v>
       </c>
       <c r="D9">
-        <v>15.48705285717237</v>
+        <v>13.84609265022454</v>
       </c>
     </row>
     <row r="10">
@@ -496,13 +496,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>14.93153046297306</v>
+        <v>10.10819953617945</v>
       </c>
       <c r="C10">
-        <v>19.90870728396405</v>
+        <v>14.03916602247153</v>
       </c>
       <c r="D10">
-        <v>19.90870728396405</v>
+        <v>14.03916602247153</v>
       </c>
     </row>
     <row r="11">
@@ -510,13 +510,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>15.56921869015158</v>
+        <v>10.04802561743162</v>
       </c>
       <c r="C11">
-        <v>19.46152336268968</v>
+        <v>13.95559113532174</v>
       </c>
       <c r="D11">
-        <v>19.46152336268968</v>
+        <v>13.95559113532174</v>
       </c>
     </row>
     <row r="12">
@@ -524,13 +524,13 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>14.2331856700339</v>
+        <v>9.964361748524935</v>
       </c>
       <c r="C12">
-        <v>15.14168688301488</v>
+        <v>13.64981061441747</v>
       </c>
       <c r="D12">
-        <v>15.14168688301488</v>
+        <v>13.64981061441747</v>
       </c>
     </row>
     <row r="13">
@@ -538,13 +538,13 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>14.90680230724399</v>
+        <v>9.935132616278832</v>
       </c>
       <c r="C13">
-        <v>16.20304598613459</v>
+        <v>13.60977070723142</v>
       </c>
       <c r="D13">
-        <v>16.20304598613459</v>
+        <v>13.60977070723142</v>
       </c>
     </row>
     <row r="14">
@@ -552,13 +552,13 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>15.22146928454996</v>
+        <v>9.877620505261458</v>
       </c>
       <c r="C14">
-        <v>16.19305243037238</v>
+        <v>13.53098699350885</v>
       </c>
       <c r="D14">
-        <v>16.19305243037238</v>
+        <v>13.53098699350885</v>
       </c>
     </row>
     <row r="15">
@@ -566,13 +566,13 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>14.75252003652782</v>
+        <v>9.730356576858799</v>
       </c>
       <c r="C15">
-        <v>14.46325493777215</v>
+        <v>14.96977934901378</v>
       </c>
       <c r="D15">
-        <v>14.46325493777215</v>
+        <v>14.96977934901378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>